<commit_message>
Reorganize code to add the Dispatcher Template samples
</commit_message>
<xml_diff>
--- a/TestData/Sample1.xlsx
+++ b/TestData/Sample1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -362,7 +362,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>

</xml_diff>